<commit_message>
working on price compariosn
</commit_message>
<xml_diff>
--- a/Data/CompareTemplate.xlsx
+++ b/Data/CompareTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Product Management\WIP Kaden\Price Comparison\tabletWebScraping\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7CD5BE-994A-4134-83E2-9BB82700F545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E56CE3B-6B96-401D-9FA1-4AD313473F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-10485" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53880" yWindow="-10485" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -377,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C19"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -389,227 +389,227 @@
     <col min="3" max="3" width="11.90625" customWidth="1"/>
     <col min="4" max="4" width="11.36328125" customWidth="1"/>
     <col min="5" max="5" width="11.453125" customWidth="1"/>
-    <col min="8" max="9" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.26953125" customWidth="1"/>
+    <col min="7" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>44312</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
         <v>44346</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
       </c>
       <c r="C3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
         <v>44822</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
       </c>
       <c r="C4">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
         <v>44312</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
       </c>
       <c r="C5">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
         <v>44346</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
       </c>
       <c r="C6">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
         <v>44822</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
         <v>44312</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
         <v>44346</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
       </c>
       <c r="C9">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
         <v>44822</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
       </c>
       <c r="C10">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
         <v>44312</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
         <v>44346</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
         <v>44822</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1">
         <v>44312</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
       </c>
       <c r="C14">
         <v>100</v>
       </c>
-      <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1">
         <v>44346</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
       </c>
       <c r="C15">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1">
         <v>44822</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
       </c>
       <c r="C16">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1">
         <v>44221</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
       </c>
       <c r="C17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1">
         <v>44637</v>
-      </c>
-      <c r="B18" t="s">
-        <v>8</v>
       </c>
       <c r="C18">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1">
         <v>44915</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
       </c>
       <c r="C19">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H22" s="2"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="I27" s="1"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H27" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>